<commit_message>
LVMH update and other
</commit_message>
<xml_diff>
--- a/PUM.DE.xlsx
+++ b/PUM.DE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.Finance\Anaylsen\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FA030D-DA27-45B3-9430-929E1D67E07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED6575A-B932-4874-A72D-CA5E69BBE28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20925" xr2:uid="{DF056538-1695-47DF-BC32-BA7DD1F9A83B}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20925" activeTab="1" xr2:uid="{DF056538-1695-47DF-BC32-BA7DD1F9A83B}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46746356-DDAA-46AE-8571-B699D0C98654}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <v>24.59</v>
+        <v>20.399999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -645,7 +645,7 @@
         <v>148.08000000000001</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -657,7 +657,7 @@
       </c>
       <c r="I4" s="3">
         <f>+I2*I3</f>
-        <v>3641.2872000000002</v>
+        <v>3020.8319999999999</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -671,7 +671,7 @@
         <v>283.89999999999998</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -683,7 +683,7 @@
         <v>1307.1999999999998</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
       </c>
       <c r="I7" s="3">
         <f>+I4-I5+I6</f>
-        <v>4664.5871999999999</v>
+        <v>4044.1319999999996</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -710,11 +710,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358FBAD2-1CB2-460A-BF2B-D7C2BA58E00E}">
   <dimension ref="A1:BH264"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1399,9 @@
       <c r="G11" s="6">
         <v>2102.3000000000002</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6">
+        <v>2117.3000000000002</v>
+      </c>
       <c r="I11" s="6">
         <v>2308.1999999999998</v>
       </c>
@@ -1409,7 +1411,9 @@
       <c r="K11" s="6">
         <v>2076</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="6">
+        <v>1942.2</v>
+      </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="3"/>
@@ -1568,7 +1572,7 @@
       </c>
       <c r="H13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2117.3000000000002</v>
       </c>
       <c r="I13" s="3">
         <f>+I11-I12</f>
@@ -1835,14 +1839,14 @@
       </c>
       <c r="H16" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2117.3000000000002</v>
       </c>
       <c r="I16" s="3">
         <f>+I13+I14-I15</f>
         <v>236.99999999999989</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" ref="J16:K18" si="4">+J13+J14-J15</f>
+        <f t="shared" ref="J16:K16" si="4">+J13+J14-J15</f>
         <v>108.90000000000009</v>
       </c>
       <c r="K16" s="3">
@@ -2022,7 +2026,7 @@
       </c>
       <c r="H18" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2117.3000000000002</v>
       </c>
       <c r="I18" s="3">
         <f t="shared" si="7"/>
@@ -2209,7 +2213,7 @@
       </c>
       <c r="H20" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2117.3000000000002</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="10"/>
@@ -2396,7 +2400,7 @@
       </c>
       <c r="H22" s="3">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>2117.3000000000002</v>
       </c>
       <c r="I22" s="3">
         <f t="shared" si="13"/>
@@ -2881,9 +2885,9 @@
         <f t="shared" si="20"/>
         <v>0.47519383532321752</v>
       </c>
-      <c r="H28" s="7" t="e">
+      <c r="H28" s="7">
         <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="I28" s="7">
         <f>+I13/I11</f>
@@ -2971,9 +2975,9 @@
         <f t="shared" si="22"/>
         <v>7.5583884317176567E-2</v>
       </c>
-      <c r="H29" s="7" t="e">
+      <c r="H29" s="7">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="I29" s="7">
         <f>+I16/I11</f>
@@ -3061,9 +3065,9 @@
         <f t="shared" si="24"/>
         <v>0.24981074943224771</v>
       </c>
-      <c r="H30" s="7" t="e">
+      <c r="H30" s="7">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="I30" s="7">
         <f>+I19/I18</f>

</xml_diff>